<commit_message>
sorted the product backlog items by priority
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\git\Capstone20\5\sprints\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CB12AD-D48E-4835-B33C-A91E159D8B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -157,84 +166,88 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -424,25 +437,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="34.71"/>
-    <col customWidth="1" min="3" max="3" width="50.29"/>
-    <col customWidth="1" min="4" max="4" width="51.43"/>
+    <col min="1" max="1" width="14.42578125" style="3"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,292 +476,295 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4">
-        <v>-1.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4">
-        <v>2.0</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24">
-      <c r="C24" s="4"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
+    <sortCondition ref="A2:A24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sprint 2 backlog during sprint 2 review
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\source\repos\CS4982CapstoneProject\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\Desktop\CS4982CapstoneProject\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC34193B-F998-4BC0-94E4-E267CD103690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046EBA04-14EC-4137-AD92-57BED784C60F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t xml:space="preserve"> I can keep members informed on their order status.</t>
   </si>
   <si>
-    <t>be able to view a detailed list of orders that are outgoing</t>
-  </si>
-  <si>
     <t xml:space="preserve"> I can easily view where current orders need to be shipped.</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t xml:space="preserve"> we always have a good inventory</t>
   </si>
   <si>
-    <t>track when things are received and shipped</t>
-  </si>
-  <si>
     <t xml:space="preserve"> we know where rentals are </t>
   </si>
   <si>
@@ -155,6 +149,12 @@
   </si>
   <si>
     <t>I can see what I want to borrow</t>
+  </si>
+  <si>
+    <t>be able to view a detailed list of orders that are outgoing/incoming</t>
+  </si>
+  <si>
+    <t>view history a single item</t>
   </si>
 </sst>
 </file>
@@ -447,14 +447,14 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="3"/>
     <col min="2" max="2" width="34.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.44140625" style="3" customWidth="1"/>
     <col min="5" max="16384" width="14.44140625" style="3"/>
   </cols>
@@ -495,10 +495,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -565,21 +565,21 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
+      <c r="B9" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>31</v>
@@ -587,30 +587,30 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -618,13 +618,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -674,13 +674,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,13 +688,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,13 +702,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -716,13 +716,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -745,8 +745,8 @@
       <c r="C23" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D26">
-    <sortCondition ref="A2:A26"/>
+  <sortState ref="A2:D23">
+    <sortCondition ref="A2:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated sprint backlog to match changes made in product backlog
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\Desktop\CS4982CapstoneProject\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\CS4982CapstoneProject\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046EBA04-14EC-4137-AD92-57BED784C60F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17A3925-97BB-4262-AFD0-7D8ED8E4F26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,19 +447,19 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3"/>
-    <col min="2" max="2" width="34.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="60.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="14.44140625" style="3"/>
+    <col min="1" max="1" width="14.42578125" style="3"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -501,7 +501,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -543,7 +543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -557,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -571,7 +571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -585,7 +585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -599,7 +599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -613,7 +613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>4</v>
       </c>
@@ -641,7 +641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -655,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>4</v>
       </c>
@@ -669,7 +669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>4</v>
       </c>
@@ -683,7 +683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -697,7 +697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>4</v>
       </c>
@@ -711,7 +711,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>4</v>
       </c>
@@ -725,27 +725,27 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D23">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
     <sortCondition ref="A2:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated backlogs Updated the sprint 3 backlog with development tasks. Updated the sprint 2 backlog to show all tasks as complete
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\College Work\CLASSES\Computing Capstone\CS4982CapstoneProject\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\CS4982CapstoneProject\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D161A93-6471-457B-B37B-77A6DB73258C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B814D-750F-493A-8476-961BB08D2370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17550" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Backlog Updated the product backlog for sprint 5
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\College Work\CLASSES\Computing Capstone\CS4982CapstoneProject\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E81326-D519-4806-A6BF-B0C0B210E2CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963F415-D621-4352-863C-71721313F22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>24</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -629,86 +629,86 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>32</v>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>4</v>
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>32</v>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>32</v>
+      <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -745,8 +745,8 @@
       <c r="C23" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
-    <sortCondition ref="A2:A23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated documentation updated the backlogs
</commit_message>
<xml_diff>
--- a/sprints/CapstoneProductBacklog.xlsx
+++ b/sprints/CapstoneProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\College Work\CLASSES\Computing Capstone\CS4982CapstoneProject\sprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\CS4982CapstoneProject\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963F415-D621-4352-863C-71721313F22A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30077CB2-8305-4A3F-8D0B-A1435DCB2F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C19" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -643,7 +643,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>32</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>32</v>
@@ -749,5 +749,6 @@
     <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>